<commit_message>
Refactoring, fixed Move command combination
</commit_message>
<xml_diff>
--- a/NNet/Docu/ConnectsTo.xlsx
+++ b/NNet/Docu/ConnectsTo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW-projects\Solutions\NNet\Docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4630EFE-1FAA-487B-B247-36F290406831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135A8509-226C-4291-8B9C-0A0667E50191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24675" yWindow="16710" windowWidth="21210" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="60">
   <si>
     <t>SRC</t>
   </si>
@@ -204,6 +204,18 @@
   </si>
   <si>
     <t>ExtendOutputLineCmd</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Constructor</t>
+  </si>
+  <si>
+    <t>Do</t>
+  </si>
+  <si>
+    <t>Undo</t>
   </si>
 </sst>
 </file>
@@ -227,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,8 +264,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -444,11 +468,175 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -486,21 +674,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -510,6 +683,52 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -518,9 +737,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFFF"/>
       <color rgb="FF71FFB1"/>
       <color rgb="FFFF0000"/>
-      <color rgb="FFFFFFFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -797,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J24"/>
+  <dimension ref="B1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -809,19 +1028,19 @@
     <col min="3" max="9" width="15.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="18" t="s">
+    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
@@ -847,7 +1066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
@@ -873,7 +1092,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
@@ -899,7 +1118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
@@ -925,7 +1144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
@@ -951,7 +1170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
@@ -977,7 +1196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
@@ -1003,7 +1222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B10" s="12" t="s">
         <v>9</v>
       </c>
@@ -1029,232 +1248,330 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B12" s="14" t="s">
+    <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="H12" t="s">
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="38" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B13" s="13" t="s">
+      <c r="J12" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="L12" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" s="41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B13" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="D13" s="31"/>
+      <c r="E13" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G13" t="s">
+      <c r="F13" s="31"/>
+      <c r="G13" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="33" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B14" s="13" t="s">
+      <c r="K13" s="34"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="42"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="D14" s="16"/>
+      <c r="E14" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G14" t="s">
+      <c r="F14" s="16"/>
+      <c r="G14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="26" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B15" s="13" t="s">
+      <c r="K14" s="28"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="20"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B15" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G15" t="s">
+      <c r="F15" s="16"/>
+      <c r="G15" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B16" s="13" t="s">
+      <c r="J15" s="26"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="20"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B16" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="D16" s="16"/>
+      <c r="E16" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G16" t="s">
+      <c r="F16" s="16"/>
+      <c r="G16" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B17" s="13" t="s">
+      <c r="J16" s="26"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="20"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="D17" s="16"/>
+      <c r="E17" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G17" t="s">
+      <c r="F17" s="16"/>
+      <c r="G17" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B18" s="13" t="s">
+      <c r="J17" s="26"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="20"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B18" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="D18" s="16"/>
+      <c r="E18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G18" t="s">
+      <c r="F18" s="16"/>
+      <c r="G18" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B19" s="15" t="s">
+      <c r="J18" s="26"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="20"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B19" s="21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B20" s="13" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="20"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B20" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E20" t="s">
+      <c r="D20" s="16"/>
+      <c r="E20" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G20" t="s">
+      <c r="F20" s="16"/>
+      <c r="G20" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="I20" t="s">
+      <c r="H20" s="16"/>
+      <c r="I20" s="16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B21" s="13" t="s">
+      <c r="J20" s="26"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="45"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B21" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E21" t="s">
+      <c r="D21" s="16"/>
+      <c r="E21" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="G21" t="s">
+      <c r="F21" s="16"/>
+      <c r="G21" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="I21" t="s">
+      <c r="H21" s="16"/>
+      <c r="I21" s="16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B22" s="13" t="s">
+      <c r="J21" s="26"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="20"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B22" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E22" t="s">
+      <c r="D22" s="16"/>
+      <c r="E22" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G22" t="s">
+      <c r="F22" s="16"/>
+      <c r="G22" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I22" t="s">
+      <c r="H22" s="16"/>
+      <c r="I22" s="16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B23" s="13" t="s">
+      <c r="J22" s="26"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="20"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B23" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E23" t="s">
+      <c r="D23" s="16"/>
+      <c r="E23" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G23" t="s">
+      <c r="F23" s="16"/>
+      <c r="G23" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I23" t="s">
+      <c r="H23" s="16"/>
+      <c r="I23" s="16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B24" s="13" t="s">
+      <c r="J23" s="26"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="20"/>
+    </row>
+    <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E24" t="s">
+      <c r="D24" s="23"/>
+      <c r="E24" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G24" t="s">
+      <c r="F24" s="23"/>
+      <c r="G24" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I24" t="s">
+      <c r="H24" s="23"/>
+      <c r="I24" s="23" t="s">
         <v>38</v>
       </c>
+      <c r="J24" s="27"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
BaseKnot completely replaced by PosNob
</commit_message>
<xml_diff>
--- a/NNet/Docu/ConnectsTo.xlsx
+++ b/NNet/Docu/ConnectsTo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW-projects\Solutions\NNet\Docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B388E2-8274-4CA7-863F-67B75265AAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8570E953-419E-4B92-9DD3-60FBA95362A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25785" yWindow="16440" windowWidth="21210" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="61">
   <si>
     <t>SRC</t>
   </si>
@@ -242,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,12 +273,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -685,8 +679,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -697,9 +689,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -709,31 +722,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1024,7 +1018,7 @@
   <dimension ref="B1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1035,39 +1029,39 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="39"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="42"/>
     </row>
     <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="39" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1075,25 +1069,25 @@
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="44" t="s">
+      <c r="C4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="36" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1119,7 +1113,7 @@
       <c r="H5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="32" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1145,7 +1139,7 @@
       <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="41" t="s">
+      <c r="I6" s="32" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1171,7 +1165,7 @@
       <c r="H7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="41" t="s">
+      <c r="I7" s="32" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1197,7 +1191,7 @@
       <c r="H8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="32" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1249,36 +1243,36 @@
       <c r="H10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="42" t="s">
+      <c r="I10" s="33" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="30" t="s">
+      <c r="I12" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="31" t="s">
+      <c r="J12" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="K12" s="32" t="s">
+      <c r="K12" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="L12" s="29" t="s">
+      <c r="L12" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="33" t="s">
+      <c r="M12" s="31" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1306,9 +1300,9 @@
       <c r="J13" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="40"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="45"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B14" s="11" t="s">
@@ -1334,9 +1328,9 @@
       <c r="J14" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="20"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="12"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="48"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B15" s="11" t="s">
@@ -1360,9 +1354,9 @@
         <v>34</v>
       </c>
       <c r="J15" s="18"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="12"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="48"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B16" s="11" t="s">
@@ -1386,9 +1380,9 @@
         <v>36</v>
       </c>
       <c r="J16" s="18"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="12"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="48"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B17" s="11" t="s">
@@ -1412,9 +1406,9 @@
         <v>37</v>
       </c>
       <c r="J17" s="18"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="12"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="48"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B18" s="11" t="s">
@@ -1438,9 +1432,9 @@
         <v>43</v>
       </c>
       <c r="J18" s="18"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="12"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="48"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B19" s="13" t="s">
@@ -1454,9 +1448,9 @@
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="18"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="12"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="48"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B20" s="11" t="s">
@@ -1480,9 +1474,9 @@
       <c r="J20" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="34"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="36"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="48"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B21" s="11" t="s">
@@ -1503,7 +1497,9 @@
       <c r="I21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="J21" s="18"/>
+      <c r="J21" s="18" t="s">
+        <v>46</v>
+      </c>
       <c r="K21" s="20"/>
       <c r="L21" s="10"/>
       <c r="M21" s="12"/>

</xml_diff>

<commit_message>
bug in ConnectCreateSynapseCmd fixed
</commit_message>
<xml_diff>
--- a/NNet/Docu/ConnectsTo.xlsx
+++ b/NNet/Docu/ConnectsTo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW-projects\Solutions\NNet\Docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3841B259-16C1-4E2A-88C2-2BFBF23DE029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559D20CD-BB96-41E6-B7B6-9CDE21518062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28035" yWindow="16875" windowWidth="25815" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27510" yWindow="16200" windowWidth="24765" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,12 +267,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -626,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -653,13 +647,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -667,7 +656,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -681,13 +669,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -730,6 +711,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1020,7 +1015,7 @@
   <dimension ref="B1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15:M15"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1031,39 +1026,39 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="39" t="s">
+      <c r="I3" s="30" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1071,25 +1066,25 @@
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="35" t="s">
+      <c r="C4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="27" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1115,7 +1110,7 @@
       <c r="H5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1141,7 +1136,7 @@
       <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1167,7 +1162,7 @@
       <c r="H7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1193,7 +1188,7 @@
       <c r="H8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1245,69 +1240,69 @@
       <c r="H10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="33" t="s">
+      <c r="I10" s="24" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26" t="s">
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="L12" s="26" t="s">
+      <c r="L12" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="30" t="s">
+      <c r="M12" s="49" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21" t="s">
+      <c r="D13" s="16"/>
+      <c r="E13" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="23"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="31"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="22"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -1327,15 +1322,15 @@
       <c r="I14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="40"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="41"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="35"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -1355,13 +1350,13 @@
       <c r="I15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="44"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="35"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -1381,13 +1376,13 @@
       <c r="I16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="40"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="8"/>
-      <c r="M16" s="41"/>
+      <c r="M16" s="32"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -1407,13 +1402,13 @@
       <c r="I17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="40"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="31"/>
       <c r="L17" s="8"/>
-      <c r="M17" s="41"/>
+      <c r="M17" s="32"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -1433,29 +1428,29 @@
       <c r="I18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="16"/>
-      <c r="K18" s="40"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="31"/>
       <c r="L18" s="8"/>
-      <c r="M18" s="41"/>
+      <c r="M18" s="32"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="41"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="44"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -1473,15 +1468,15 @@
       <c r="I20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="J20" s="16" t="s">
+      <c r="J20" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="42"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="44"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="35"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -1499,15 +1494,15 @@
       <c r="I21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="J21" s="16" t="s">
+      <c r="J21" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="12"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="35"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -1525,13 +1520,13 @@
       <c r="I22" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J22" s="16"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="12"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="35"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -1549,34 +1544,34 @@
       <c r="I23" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="44"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="35"/>
     </row>
     <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15" t="s">
+      <c r="D24" s="12"/>
+      <c r="E24" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15" t="s">
+      <c r="F24" s="12"/>
+      <c r="G24" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15" t="s">
+      <c r="H24" s="12"/>
+      <c r="I24" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="17"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="47"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
PLugIoLineAnimation removed, now without animation. Running.
</commit_message>
<xml_diff>
--- a/NNet/Docu/ConnectsTo.xlsx
+++ b/NNet/Docu/ConnectsTo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW-projects\Solutions\NNet\Docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559D20CD-BB96-41E6-B7B6-9CDE21518062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41171D4-F680-4730-8355-87FD4D7110EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27510" yWindow="16200" windowWidth="24765" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27435" yWindow="16875" windowWidth="24765" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -702,15 +702,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -725,6 +716,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1015,7 +1015,7 @@
   <dimension ref="B1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1026,15 +1026,15 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="41"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="51"/>
     </row>
     <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="5" t="s">
@@ -1249,27 +1249,27 @@
       <c r="B12" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45" t="s">
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="46" t="s">
+      <c r="I12" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="47" t="s">
+      <c r="J12" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="K12" s="48" t="s">
+      <c r="K12" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="L12" s="45" t="s">
+      <c r="L12" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="49" t="s">
+      <c r="M12" s="46" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1377,9 +1377,9 @@
         <v>36</v>
       </c>
       <c r="J16" s="13"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="32"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="35"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B17" s="10" t="s">
@@ -1403,9 +1403,9 @@
         <v>37</v>
       </c>
       <c r="J17" s="13"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="32"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="35"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B18" s="10" t="s">
@@ -1434,20 +1434,20 @@
       <c r="M18" s="32"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="41"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B20" s="10" t="s">

</xml_diff>

<commit_message>
work on Nob input/output
</commit_message>
<xml_diff>
--- a/NNet/Docu/ConnectsTo.xlsx
+++ b/NNet/Docu/ConnectsTo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW-projects\Solutions\NNet\Docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41171D4-F680-4730-8355-87FD4D7110EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A8DD34-2409-4542-8921-9DB3AD27AD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27435" yWindow="16875" windowWidth="24765" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36763" yWindow="2357" windowWidth="23606" windowHeight="14803" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -98,9 +98,6 @@
     <t>(5)</t>
   </si>
   <si>
-    <t>PlugIoLineAnimation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Drag source Nob to destination Nob: </t>
   </si>
   <si>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t>ConnectCreateSynapseCmd</t>
+  </si>
+  <si>
+    <t>PlugIoLine</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1015,7 @@
   <dimension ref="B1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1247,7 +1247,7 @@
     <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B12" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="42"/>
       <c r="D12" s="42"/>
@@ -1261,16 +1261,16 @@
         <v>1</v>
       </c>
       <c r="J12" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="K12" s="45" t="s">
+      <c r="L12" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="L12" s="42" t="s">
+      <c r="M12" s="46" t="s">
         <v>57</v>
-      </c>
-      <c r="M12" s="46" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.4">
@@ -1278,24 +1278,24 @@
         <v>15</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>40</v>
-      </c>
       <c r="J13" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K13" s="19"/>
       <c r="L13" s="20"/>
@@ -1306,24 +1306,24 @@
         <v>16</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="J14" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K14" s="19"/>
       <c r="L14" s="20"/>
@@ -1334,21 +1334,21 @@
         <v>17</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="33"/>
@@ -1360,21 +1360,21 @@
         <v>18</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J16" s="13"/>
       <c r="K16" s="33"/>
@@ -1386,21 +1386,21 @@
         <v>19</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="33"/>
@@ -1409,24 +1409,24 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="31"/>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B19" s="47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="40"/>
@@ -1451,25 +1451,25 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B20" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K20" s="33"/>
       <c r="L20" s="34"/>
@@ -1477,25 +1477,25 @@
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B21" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K21" s="33"/>
       <c r="L21" s="34"/>
@@ -1503,22 +1503,22 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B22" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J22" s="13"/>
       <c r="K22" s="33"/>
@@ -1527,22 +1527,22 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B23" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J23" s="13"/>
       <c r="K23" s="33"/>
@@ -1551,22 +1551,22 @@
     </row>
     <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J24" s="14"/>
       <c r="K24" s="36"/>

</xml_diff>

<commit_message>
Connect IoLines and IoConnectors. Running.
</commit_message>
<xml_diff>
--- a/NNet/Docu/ConnectsTo.xlsx
+++ b/NNet/Docu/ConnectsTo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW-projects\Solutions\NNet\Docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD52DC9C-92F2-4C06-9AFD-A73A8DE8FE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B756BC1-159F-4674-BF9D-2785CCF8D752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26385" yWindow="16995" windowWidth="23610" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35049" yWindow="1037" windowWidth="23922" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="70">
   <si>
     <t>SRC</t>
   </si>
@@ -219,6 +219,33 @@
   </si>
   <si>
     <t>AddSynapse</t>
+  </si>
+  <si>
+    <t>input connector (12)</t>
+  </si>
+  <si>
+    <t>output connector (13)</t>
+  </si>
+  <si>
+    <t>(12)</t>
+  </si>
+  <si>
+    <t>(13)</t>
+  </si>
+  <si>
+    <t>InputConnector</t>
+  </si>
+  <si>
+    <t>OutputConnector</t>
+  </si>
+  <si>
+    <t>input connector</t>
+  </si>
+  <si>
+    <t>output connector</t>
+  </si>
+  <si>
+    <t>ConnAnimationCommand</t>
   </si>
 </sst>
 </file>
@@ -268,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -298,51 +325,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -605,125 +587,180 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1012,87 +1049,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M24"/>
+  <dimension ref="B2:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="12.765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="15.69140625" customWidth="1"/>
+    <col min="3" max="11" width="15.69140625" customWidth="1"/>
+    <col min="12" max="12" width="15.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="51"/>
-    </row>
-    <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="44" t="s">
         <v>9</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="44" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="26" t="s">
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="48" t="s">
         <v>11</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1111,6 +1162,12 @@
         <v>5</v>
       </c>
       <c r="I5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1118,7 +1175,7 @@
       <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1137,6 +1194,12 @@
         <v>5</v>
       </c>
       <c r="I6" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1144,7 +1207,7 @@
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1163,6 +1226,12 @@
         <v>5</v>
       </c>
       <c r="I7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1170,7 +1239,7 @@
       <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1189,6 +1258,12 @@
         <v>12</v>
       </c>
       <c r="I8" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1196,7 +1271,7 @@
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1211,18 +1286,24 @@
       <c r="G9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>5</v>
+      <c r="H9" s="39" t="s">
+        <v>61</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="49" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -1240,127 +1321,143 @@
       <c r="H10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="21" t="s">
+      <c r="I10" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42" t="s">
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="43" t="s">
+      <c r="I14" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="44" t="s">
+      <c r="J14" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="45" t="s">
+      <c r="K14" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="L12" s="42" t="s">
+      <c r="L14" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="M12" s="46" t="s">
+      <c r="M14" s="36" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B13" s="15" t="s">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C15" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16" t="s">
+      <c r="F15" s="16"/>
+      <c r="G15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H15" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I15" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="19"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="22"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14" s="19"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="35"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="35"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="22"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B16" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="9" t="s">
@@ -1374,19 +1471,21 @@
         <v>35</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="35"/>
+        <v>38</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="19"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="28"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B17" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="9" t="s">
@@ -1400,19 +1499,19 @@
         <v>34</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J17" s="13"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="35"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="28"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B18" s="10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="9" t="s">
@@ -1423,159 +1522,267 @@
         <v>37</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J18" s="13"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="32"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="28"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B19" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="41"/>
+      <c r="B19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="28"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B20" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="8" t="s">
-        <v>30</v>
+      <c r="E20" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="I20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="K20" s="33"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="35"/>
+        <v>39</v>
+      </c>
+      <c r="J20" s="13"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="25"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B21" s="10" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="D21" s="8"/>
-      <c r="E21" s="8" t="s">
-        <v>60</v>
+      <c r="E21" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K21" s="24"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="25"/>
+    </row>
+    <row r="22" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K22" s="24"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="25"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B23" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="31"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B24" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K24" s="26"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="28"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8" t="s">
+      <c r="H25" s="8"/>
+      <c r="I25" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J25" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="K21" s="33"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="35"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B22" s="10" t="s">
+      <c r="K25" s="26"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="28"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B26" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8" t="s">
+      <c r="D26" s="8"/>
+      <c r="E26" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8" t="s">
+      <c r="F26" s="8"/>
+      <c r="G26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8" t="s">
+      <c r="H26" s="8"/>
+      <c r="I26" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="35"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B23" s="10" t="s">
+      <c r="J26" s="13"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="28"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B27" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C27" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8" t="s">
+      <c r="D27" s="8"/>
+      <c r="E27" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8" t="s">
+      <c r="F27" s="8"/>
+      <c r="G27" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8" t="s">
+      <c r="H27" s="8"/>
+      <c r="I27" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="35"/>
-    </row>
-    <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="11" t="s">
+      <c r="J27" s="13"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="28"/>
+    </row>
+    <row r="28" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C28" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12" t="s">
+      <c r="D28" s="12"/>
+      <c r="E28" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12" t="s">
+      <c r="F28" s="12"/>
+      <c r="G28" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12" t="s">
+      <c r="H28" s="12"/>
+      <c r="I28" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="38"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="C2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
work on IoConnector direction and rotation. Much better, but still smaller bug.
</commit_message>
<xml_diff>
--- a/NNet/Docu/ConnectsTo.xlsx
+++ b/NNet/Docu/ConnectsTo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW-projects\Solutions\NNet\Docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B756BC1-159F-4674-BF9D-2785CCF8D752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E3C37E-BE95-4A10-AD6B-64ACDB6A4495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35049" yWindow="1037" windowWidth="23922" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4003" yWindow="849" windowWidth="21600" windowHeight="15677" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -269,7 +269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,6 +294,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -657,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -732,34 +738,37 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1052,7 +1061,7 @@
   <dimension ref="B2:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1063,47 +1072,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="42" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1126,10 +1135,10 @@
       <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="48" t="s">
+      <c r="I4" s="46" t="s">
         <v>11</v>
       </c>
       <c r="J4" s="23" t="s">
@@ -1158,11 +1167,11 @@
       <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>5</v>
+      <c r="H5" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="J5" s="23" t="s">
         <v>5</v>
@@ -1274,8 +1283,8 @@
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>5</v>
+      <c r="D9" s="50" t="s">
+        <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>5</v>
@@ -1303,11 +1312,11 @@
       <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>5</v>
+      <c r="C10" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>5</v>
@@ -1332,10 +1341,10 @@
       </c>
     </row>
     <row r="11" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="47" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1364,10 +1373,10 @@
       </c>
     </row>
     <row r="12" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="47" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="3" t="s">

</xml_diff>

<commit_message>
New concept for Synapse implemented
</commit_message>
<xml_diff>
--- a/NNet/Docu/ConnectsTo.xlsx
+++ b/NNet/Docu/ConnectsTo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW-projects\Solutions\NNet\Docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E3C37E-BE95-4A10-AD6B-64ACDB6A4495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8E85D1-3F4E-4A8E-9F2F-95E8995969B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4003" yWindow="849" windowWidth="21600" windowHeight="15677" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39977" yWindow="626" windowWidth="19389" windowHeight="15677" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -762,14 +762,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1061,7 +1061,7 @@
   <dimension ref="B2:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1072,17 +1072,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
@@ -1167,10 +1167,10 @@
       <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="50" t="s">
+      <c r="H5" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="50" t="s">
+      <c r="I5" s="48" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="23" t="s">
@@ -1283,7 +1283,7 @@
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="48" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1315,7 +1315,7 @@
       <c r="C10" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="48" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="3" t="s">

</xml_diff>

<commit_message>
bug in ConnectionResult fixed
</commit_message>
<xml_diff>
--- a/NNet/Docu/ConnectsTo.xlsx
+++ b/NNet/Docu/ConnectsTo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SW-projects\Solutions\NNet\Docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8E85D1-3F4E-4A8E-9F2F-95E8995969B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DAD99F-63F6-410A-9E8A-987B01318BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39977" yWindow="626" windowWidth="19389" windowHeight="15677" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33711" yWindow="206" windowWidth="25603" windowHeight="16808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="79">
   <si>
     <t>SRC</t>
   </si>
@@ -246,6 +246,33 @@
   </si>
   <si>
     <t>ConnAnimationCommand</t>
+  </si>
+  <si>
+    <t>(14)</t>
+  </si>
+  <si>
+    <t>(15)</t>
+  </si>
+  <si>
+    <t>input connector (14)</t>
+  </si>
+  <si>
+    <t>output connector (15)</t>
+  </si>
+  <si>
+    <t>(16)</t>
+  </si>
+  <si>
+    <t>(17)</t>
+  </si>
+  <si>
+    <t>input connector (16)</t>
+  </si>
+  <si>
+    <t>output connector (17)</t>
+  </si>
+  <si>
+    <t>array of knots     (6)</t>
   </si>
 </sst>
 </file>
@@ -1058,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M28"/>
+  <dimension ref="B2:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1360,16 +1387,16 @@
         <v>5</v>
       </c>
       <c r="H11" s="39" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>5</v>
+        <v>76</v>
+      </c>
+      <c r="K11" s="39" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1395,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="I12" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>5</v>
+        <v>73</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>78</v>
       </c>
       <c r="K12" s="39" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
@@ -1650,144 +1677,256 @@
       <c r="M22" s="25"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B23" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="31"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B24" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="8"/>
+      <c r="B23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K23" s="24"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="25"/>
+    </row>
+    <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B24" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="12"/>
       <c r="G24" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="28"/>
+        <v>37</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K24" s="24"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="25"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B25" s="10" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="D25" s="8"/>
-      <c r="E25" s="8" t="s">
-        <v>60</v>
+      <c r="E25" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K25" s="24"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="25"/>
+    </row>
+    <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B26" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K26" s="24"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="25"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B27" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="31"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J25" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="K25" s="26"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="28"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B26" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J26" s="13"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="28"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B27" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J27" s="13"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="28"/>
-    </row>
-    <row r="28" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" s="13"/>
+      <c r="J28" s="13" t="s">
+        <v>41</v>
+      </c>
       <c r="K28" s="26"/>
       <c r="L28" s="27"/>
       <c r="M28" s="28"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B29" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K29" s="26"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="28"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B30" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="13"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="28"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B31" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31" s="13"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="28"/>
+    </row>
+    <row r="32" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J32" s="13"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>